<commit_message>
before changing ndf part in frontend
</commit_message>
<xml_diff>
--- a/assets/latest data/Categorized Feeds 2-1 (1) Cleaned_104707 (2).xlsx
+++ b/assets/latest data/Categorized Feeds 2-1 (1) Cleaned_104707 (2).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Composition Sheet" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="66">
   <si>
     <t>Category 1</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>ME raw</t>
+  </si>
+  <si>
+    <t>NDF</t>
+  </si>
+  <si>
+    <t>Rapeseed Cake</t>
   </si>
 </sst>
 </file>
@@ -1655,10 +1661,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,7 +1672,7 @@
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -1677,28 +1683,31 @@
         <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1709,29 +1718,32 @@
         <v>23.5</v>
       </c>
       <c r="D2">
+        <v>44.1</v>
+      </c>
+      <c r="E2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E40" si="0">D2*1000</f>
+      <c r="F2">
+        <f t="shared" ref="F2:F40" si="0">E2*1000</f>
         <v>2300</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.1</v>
       </c>
-      <c r="H2">
-        <v>0.5</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="I2">
+        <v>0.6</v>
+      </c>
+      <c r="J2" s="1">
         <v>0.1</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1742,29 +1754,32 @@
         <v>8.9</v>
       </c>
       <c r="D3">
+        <v>59.5</v>
+      </c>
+      <c r="E3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.1</v>
       </c>
-      <c r="H3">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="I3">
+        <v>0.6</v>
+      </c>
+      <c r="J3" s="1">
         <v>0.1</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1775,29 +1790,32 @@
         <v>14.2</v>
       </c>
       <c r="D4">
+        <v>51.4</v>
+      </c>
+      <c r="E4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>2300</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.1</v>
       </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="I4">
+        <v>0.6</v>
+      </c>
+      <c r="J4" s="1">
         <v>0.1</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1808,29 +1826,32 @@
         <v>23</v>
       </c>
       <c r="D5">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="E5">
         <v>2.1</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>5</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.1</v>
       </c>
-      <c r="H5">
-        <v>0.5</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="I5">
+        <v>0.4</v>
+      </c>
+      <c r="J5" s="1">
         <v>0.1</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1841,29 +1862,32 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="D6">
+        <v>58.5</v>
+      </c>
+      <c r="E6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>2300</v>
       </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
       <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
         <v>0.1</v>
       </c>
-      <c r="H6">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="I6">
+        <v>0.6</v>
+      </c>
+      <c r="J6" s="1">
         <v>0.1</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1874,29 +1898,32 @@
         <v>4</v>
       </c>
       <c r="D7">
+        <v>51.1</v>
+      </c>
+      <c r="E7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.1</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.5</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>0.1</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1907,29 +1934,32 @@
         <v>6.4</v>
       </c>
       <c r="D8">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="E8">
         <v>1.7</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>1700</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>3</v>
       </c>
-      <c r="G8">
+      <c r="H8">
+        <v>0.05</v>
+      </c>
+      <c r="I8">
         <v>0.1</v>
       </c>
-      <c r="H8">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.05</v>
-      </c>
       <c r="J8" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K8" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1940,29 +1970,32 @@
         <v>11.6</v>
       </c>
       <c r="D9">
+        <v>62.5</v>
+      </c>
+      <c r="E9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>2300</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>5</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.1</v>
       </c>
-      <c r="H9">
-        <v>0.5</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="I9">
+        <v>0.4</v>
+      </c>
+      <c r="J9" s="1">
         <v>0.1</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1973,29 +2006,32 @@
         <v>4.8</v>
       </c>
       <c r="D10">
+        <v>71.8</v>
+      </c>
+      <c r="E10">
         <v>1.5</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>17</v>
       </c>
-      <c r="G10">
+      <c r="H10">
+        <v>0.01</v>
+      </c>
+      <c r="I10">
         <v>0.1</v>
       </c>
-      <c r="H10">
-        <v>0.5</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>0.01</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2006,29 +2042,32 @@
         <v>5.5</v>
       </c>
       <c r="D11">
+        <v>66.5</v>
+      </c>
+      <c r="E11">
         <v>1.7</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <f t="shared" si="0"/>
         <v>1700</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>8</v>
       </c>
-      <c r="G11">
+      <c r="H11">
+        <v>0.01</v>
+      </c>
+      <c r="I11">
         <v>0.1</v>
       </c>
-      <c r="H11">
-        <v>0.5</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>0.01</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2039,29 +2078,32 @@
         <v>4</v>
       </c>
       <c r="D12">
+        <v>72.2</v>
+      </c>
+      <c r="E12">
         <v>1.5</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>5</v>
       </c>
-      <c r="G12">
+      <c r="H12">
+        <v>0.01</v>
+      </c>
+      <c r="I12">
         <v>0.1</v>
       </c>
-      <c r="H12">
-        <v>0.5</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>0.01</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2072,29 +2114,32 @@
         <v>6.2</v>
       </c>
       <c r="D13">
+        <v>70.2</v>
+      </c>
+      <c r="E13">
         <v>1.5</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>5</v>
       </c>
-      <c r="G13">
+      <c r="H13">
+        <v>0.01</v>
+      </c>
+      <c r="I13">
         <v>0.1</v>
       </c>
-      <c r="H13">
-        <v>0.5</v>
-      </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>0.01</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2105,29 +2150,32 @@
         <v>6.6</v>
       </c>
       <c r="D14">
+        <v>68.3</v>
+      </c>
+      <c r="E14">
         <v>1.8</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>5</v>
       </c>
-      <c r="G14">
+      <c r="H14">
+        <v>0.01</v>
+      </c>
+      <c r="I14">
         <v>0.1</v>
       </c>
-      <c r="H14">
-        <v>0.5</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>0.01</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2138,29 +2186,32 @@
         <v>3.7</v>
       </c>
       <c r="D15">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="E15">
         <v>1.9</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>5</v>
       </c>
-      <c r="G15">
+      <c r="H15">
+        <v>0.01</v>
+      </c>
+      <c r="I15">
         <v>0.1</v>
       </c>
-      <c r="H15">
-        <v>0.5</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>0.01</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2171,29 +2222,32 @@
         <v>3.9</v>
       </c>
       <c r="D16">
+        <v>63.7</v>
+      </c>
+      <c r="E16">
         <v>1.5</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>15</v>
       </c>
-      <c r="G16">
+      <c r="H16">
+        <v>0.01</v>
+      </c>
+      <c r="I16">
         <v>0.1</v>
       </c>
-      <c r="H16">
-        <v>0.5</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>0.01</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2204,29 +2258,32 @@
         <v>9.1</v>
       </c>
       <c r="D17">
+        <v>10.6</v>
+      </c>
+      <c r="E17">
         <v>3.2</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>75</v>
       </c>
-      <c r="G17">
-        <v>0.1</v>
-      </c>
       <c r="H17">
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I17">
+        <v>0.3</v>
       </c>
       <c r="J17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K17" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2237,29 +2294,32 @@
         <v>14.4</v>
       </c>
       <c r="D18">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E18">
         <v>3.2</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>100</v>
       </c>
-      <c r="G18">
-        <v>0.1</v>
-      </c>
       <c r="H18">
-        <v>0.5</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I18">
+        <v>0.2</v>
       </c>
       <c r="J18" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K18" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2270,29 +2330,32 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D19">
+        <v>11.2</v>
+      </c>
+      <c r="E19">
         <v>3.1</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <f t="shared" si="0"/>
         <v>3100</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>100</v>
       </c>
-      <c r="G19">
-        <v>0.1</v>
-      </c>
       <c r="H19">
-        <v>0.5</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I19">
+        <v>0.2</v>
       </c>
       <c r="J19" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K19" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -2303,29 +2366,32 @@
         <v>12.8</v>
       </c>
       <c r="D20">
+        <v>22.4</v>
+      </c>
+      <c r="E20">
         <v>2.9</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <f t="shared" si="0"/>
         <v>2900</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>50</v>
       </c>
-      <c r="G20">
-        <v>0.1</v>
-      </c>
       <c r="H20">
-        <v>0.5</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I20">
+        <v>0.2</v>
       </c>
       <c r="J20" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K20" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2336,29 +2402,32 @@
         <v>10</v>
       </c>
       <c r="D21">
+        <v>40.5</v>
+      </c>
+      <c r="E21">
         <v>2.6</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <f t="shared" si="0"/>
         <v>2600</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>50</v>
       </c>
-      <c r="G21">
-        <v>0.1</v>
-      </c>
       <c r="H21">
-        <v>0.5</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I21">
+        <v>0.3</v>
       </c>
       <c r="J21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K21" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2369,29 +2438,32 @@
         <v>15.9</v>
       </c>
       <c r="D22">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E22">
         <v>2.8</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>45</v>
       </c>
-      <c r="G22">
-        <v>0.1</v>
-      </c>
       <c r="H22">
-        <v>0.5</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I22">
+        <v>0.3</v>
       </c>
       <c r="J22" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K22" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2402,29 +2474,32 @@
         <v>15.9</v>
       </c>
       <c r="D23">
+        <v>24.7</v>
+      </c>
+      <c r="E23">
         <v>2.8</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>30</v>
       </c>
-      <c r="G23">
-        <v>0.1</v>
-      </c>
       <c r="H23">
-        <v>0.5</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I23">
+        <v>0.3</v>
       </c>
       <c r="J23" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K23" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -2435,29 +2510,32 @@
         <v>10.7</v>
       </c>
       <c r="D24">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="E24">
         <v>2.4</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>50</v>
       </c>
-      <c r="G24">
-        <v>0.1</v>
-      </c>
       <c r="H24">
-        <v>0.5</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I24">
+        <v>0.3</v>
       </c>
       <c r="J24" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K24" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -2468,29 +2546,32 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D25">
+        <v>53.5</v>
+      </c>
+      <c r="E25">
         <v>2.1</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>20</v>
       </c>
-      <c r="G25">
+      <c r="H25">
+        <v>0.05</v>
+      </c>
+      <c r="I25">
         <v>0.1</v>
       </c>
-      <c r="H25">
-        <v>0.5</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0.05</v>
-      </c>
       <c r="J25" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K25" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2501,29 +2582,32 @@
         <v>10.3</v>
       </c>
       <c r="D26">
+        <v>28.1</v>
+      </c>
+      <c r="E26">
         <v>2.5</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>20</v>
       </c>
-      <c r="G26">
+      <c r="H26">
+        <v>0.05</v>
+      </c>
+      <c r="I26">
         <v>0.1</v>
       </c>
-      <c r="H26">
-        <v>0.5</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0.05</v>
-      </c>
       <c r="J26" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K26" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -2534,29 +2618,32 @@
         <v>15.3</v>
       </c>
       <c r="D27">
+        <v>26.8</v>
+      </c>
+      <c r="E27">
         <v>2.4</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>65</v>
       </c>
-      <c r="G27">
-        <v>0.1</v>
-      </c>
       <c r="H27">
-        <v>0.5</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I27">
+        <v>0.2</v>
       </c>
       <c r="J27" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K27" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -2567,29 +2654,32 @@
         <v>16.8</v>
       </c>
       <c r="D28">
+        <v>31.6</v>
+      </c>
+      <c r="E28">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <f t="shared" si="0"/>
         <v>2300</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>65</v>
       </c>
-      <c r="G28">
-        <v>0.1</v>
-      </c>
       <c r="H28">
-        <v>0.5</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I28">
+        <v>0.2</v>
       </c>
       <c r="J28" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K28" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -2600,29 +2690,32 @@
         <v>17.5</v>
       </c>
       <c r="D29">
+        <v>28.6</v>
+      </c>
+      <c r="E29">
         <v>2.5</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>65</v>
       </c>
-      <c r="G29">
-        <v>0.1</v>
-      </c>
       <c r="H29">
-        <v>0.5</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I29">
+        <v>0.2</v>
       </c>
       <c r="J29" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K29" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -2633,29 +2726,32 @@
         <v>3.5</v>
       </c>
       <c r="D30">
+        <v>27.4</v>
+      </c>
+      <c r="E30">
         <v>2.5</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>20</v>
       </c>
-      <c r="G30">
-        <v>0.1</v>
-      </c>
       <c r="H30">
-        <v>0.5</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I30">
+        <v>0.09</v>
       </c>
       <c r="J30" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K30" s="1">
         <v>0.09</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2666,29 +2762,32 @@
         <v>78.599999999999994</v>
       </c>
       <c r="D31">
+        <v>13.3</v>
+      </c>
+      <c r="E31">
         <v>2.8</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>20</v>
       </c>
-      <c r="G31">
-        <v>0.1</v>
-      </c>
       <c r="H31">
-        <v>0.5</v>
-      </c>
-      <c r="I31" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I31">
+        <v>0.2</v>
       </c>
       <c r="J31" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K31" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -2699,29 +2798,32 @@
         <v>23.8</v>
       </c>
       <c r="D32">
+        <v>43.2</v>
+      </c>
+      <c r="E32">
         <v>2</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>100</v>
       </c>
-      <c r="G32">
-        <v>0.1</v>
-      </c>
       <c r="H32">
-        <v>0.5</v>
-      </c>
-      <c r="I32" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I32">
+        <v>0.2</v>
       </c>
       <c r="J32" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K32" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -2732,29 +2834,32 @@
         <v>48</v>
       </c>
       <c r="D33">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E33">
         <v>2.1</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>300</v>
       </c>
-      <c r="G33">
-        <v>0.1</v>
-      </c>
       <c r="H33">
-        <v>0.5</v>
-      </c>
-      <c r="I33" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I33">
+        <v>0.3</v>
       </c>
       <c r="J33" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K33" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -2765,31 +2870,34 @@
         <v>39.6</v>
       </c>
       <c r="D34">
+        <v>31.2</v>
+      </c>
+      <c r="E34">
         <v>2.5</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>145</v>
       </c>
-      <c r="G34">
-        <v>0.1</v>
-      </c>
       <c r="H34">
-        <v>0.5</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I34">
+        <v>0.25</v>
       </c>
       <c r="J34" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K34" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="B35">
         <v>89.9</v>
@@ -2798,29 +2906,32 @@
         <v>34.299999999999997</v>
       </c>
       <c r="D35">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E35">
         <v>2.7</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <f t="shared" si="0"/>
         <v>2700</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>130</v>
       </c>
-      <c r="G35">
-        <v>0.1</v>
-      </c>
       <c r="H35">
-        <v>0.5</v>
-      </c>
-      <c r="I35" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I35">
+        <v>0.25</v>
       </c>
       <c r="J35" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K35" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -2831,29 +2942,32 @@
         <v>29</v>
       </c>
       <c r="D36">
+        <v>30.6</v>
+      </c>
+      <c r="E36">
         <v>2.8</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>61</v>
       </c>
-      <c r="G36">
-        <v>0.1</v>
-      </c>
       <c r="H36">
-        <v>0.5</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I36">
+        <v>0.25</v>
       </c>
       <c r="J36" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K36" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2864,29 +2978,32 @@
         <v>59.7</v>
       </c>
       <c r="D37">
+        <v>18</v>
+      </c>
+      <c r="E37">
         <v>2.8</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>40</v>
       </c>
-      <c r="G37">
-        <v>0.1</v>
-      </c>
       <c r="H37">
-        <v>0.5</v>
-      </c>
-      <c r="I37" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I37">
+        <v>0.25</v>
       </c>
       <c r="J37" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K37" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -2897,29 +3014,32 @@
         <v>17.8</v>
       </c>
       <c r="D38">
+        <v>57</v>
+      </c>
+      <c r="E38">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>50</v>
       </c>
-      <c r="G38">
-        <v>0.1</v>
-      </c>
       <c r="H38">
-        <v>0.5</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I38">
+        <v>0.25</v>
       </c>
       <c r="J38" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K38" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -2930,29 +3050,32 @@
         <v>32.5</v>
       </c>
       <c r="D39">
+        <v>43.8</v>
+      </c>
+      <c r="E39">
         <v>2.1</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>55</v>
       </c>
-      <c r="G39">
-        <v>0.1</v>
-      </c>
       <c r="H39">
-        <v>0.5</v>
-      </c>
-      <c r="I39" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I39">
+        <v>0.25</v>
       </c>
       <c r="J39" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K39" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -2963,25 +3086,28 @@
         <v>40.4</v>
       </c>
       <c r="D40">
+        <v>56.8</v>
+      </c>
+      <c r="E40">
         <v>2.7</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <f t="shared" si="0"/>
         <v>2700</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>120</v>
       </c>
-      <c r="G40">
-        <v>0.1</v>
-      </c>
       <c r="H40">
-        <v>0.5</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0.05</v>
+        <v>0.05</v>
+      </c>
+      <c r="I40">
+        <v>0.25</v>
       </c>
       <c r="J40" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K40" s="1">
         <v>0.25</v>
       </c>
     </row>
@@ -3883,7 +4009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
corrected the results with updated data of changing inclusion levels to 20% of Sarson, Mott Grss and Barseem
</commit_message>
<xml_diff>
--- a/assets/latest data/Categorized Feeds 2-1 (1) Cleaned_104707 (2).xlsx
+++ b/assets/latest data/Categorized Feeds 2-1 (1) Cleaned_104707 (2).xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\donewithit\assets\latest data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Composition Sheet"/>
-    <sheet r:id="rId2" sheetId="2" name="clean composition"/>
-    <sheet r:id="rId3" sheetId="3" name="NDF Added with updated Inclusio"/>
-    <sheet r:id="rId4" sheetId="4" name="Sheet1"/>
-    <sheet r:id="rId5" sheetId="5" name="Translation"/>
+    <sheet name="Composition Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="clean composition" sheetId="2" r:id="rId2"/>
+    <sheet name="Composition April 6, 2023" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="66">
   <si>
     <t>Barseem</t>
   </si>
@@ -221,8 +225,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,7 +250,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -261,16 +264,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -285,65 +288,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -354,10 +351,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -395,71 +392,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -487,7 +484,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -510,11 +507,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -523,13 +520,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -539,7 +536,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -548,7 +545,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -557,7 +554,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -565,10 +562,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -639,21 +636,20 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="86" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="31.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="6.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="6.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="31.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>57</v>
       </c>
@@ -679,7 +675,7 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,10 +686,11 @@
         <v>23.5</v>
       </c>
       <c r="D2" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E2" s="7">
-        <f>D2*1000</f>
+        <f t="shared" ref="E2:E40" si="0">D2*1000</f>
+        <v>2300</v>
       </c>
       <c r="F2" s="7">
         <v>5</v>
@@ -705,7 +702,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -716,10 +713,11 @@
         <v>8.9</v>
       </c>
       <c r="D3" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E3" s="7">
-        <f>D3*1000</f>
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="F3" s="7">
         <v>5</v>
@@ -731,7 +729,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -742,10 +740,11 @@
         <v>14.2</v>
       </c>
       <c r="D4" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E4" s="7">
-        <f>D4*1000</f>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="F4" s="7">
         <v>5</v>
@@ -757,7 +756,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -771,7 +770,8 @@
         <v>2.1</v>
       </c>
       <c r="E5" s="7">
-        <f>D5*1000</f>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="F5" s="7">
         <v>5</v>
@@ -783,7 +783,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -791,13 +791,14 @@
         <v>29.6</v>
       </c>
       <c r="C6" s="6">
-        <v>9.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D6" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E6" s="7">
-        <f>D6*1000</f>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="F6" s="7">
         <v>10</v>
@@ -809,7 +810,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -820,10 +821,11 @@
         <v>4</v>
       </c>
       <c r="D7" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E7" s="7">
-        <f>D7*1000</f>
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="F7" s="7">
         <v>5</v>
@@ -835,7 +837,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -849,7 +851,8 @@
         <v>1.7</v>
       </c>
       <c r="E8" s="7">
-        <f>D8*1000</f>
+        <f t="shared" si="0"/>
+        <v>1700</v>
       </c>
       <c r="F8" s="7">
         <v>3</v>
@@ -861,21 +864,22 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C9" s="6">
         <v>11.6</v>
       </c>
       <c r="D9" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E9" s="7">
-        <f>D9*1000</f>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="F9" s="7">
         <v>5</v>
@@ -887,7 +891,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -901,7 +905,8 @@
         <v>1.5</v>
       </c>
       <c r="E10" s="7">
-        <f>D10*1000</f>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F10" s="7">
         <v>17</v>
@@ -913,7 +918,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -927,7 +932,8 @@
         <v>1.7</v>
       </c>
       <c r="E11" s="7">
-        <f>D11*1000</f>
+        <f t="shared" si="0"/>
+        <v>1700</v>
       </c>
       <c r="F11" s="7">
         <v>8</v>
@@ -939,7 +945,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -953,7 +959,8 @@
         <v>1.5</v>
       </c>
       <c r="E12" s="7">
-        <f>D12*1000</f>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F12" s="7">
         <v>5</v>
@@ -965,7 +972,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -979,7 +986,8 @@
         <v>1.5</v>
       </c>
       <c r="E13" s="7">
-        <f>D13*1000</f>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F13" s="7">
         <v>5</v>
@@ -991,7 +999,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1005,7 +1013,8 @@
         <v>1.8</v>
       </c>
       <c r="E14" s="7">
-        <f>D14*1000</f>
+        <f t="shared" si="0"/>
+        <v>1800</v>
       </c>
       <c r="F14" s="7">
         <v>5</v>
@@ -1017,7 +1026,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1031,7 +1040,8 @@
         <v>1.9</v>
       </c>
       <c r="E15" s="7">
-        <f>D15*1000</f>
+        <f t="shared" si="0"/>
+        <v>1900</v>
       </c>
       <c r="F15" s="7">
         <v>5</v>
@@ -1043,7 +1053,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1057,7 +1067,8 @@
         <v>1.5</v>
       </c>
       <c r="E16" s="7">
-        <f>D16*1000</f>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F16" s="7">
         <v>15</v>
@@ -1069,7 +1080,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1094,8 @@
         <v>3.2</v>
       </c>
       <c r="E17" s="7">
-        <f>D17*1000</f>
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="F17" s="7">
         <v>75</v>
@@ -1095,7 +1107,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1109,7 +1121,8 @@
         <v>3.2</v>
       </c>
       <c r="E18" s="7">
-        <f>D18*1000</f>
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="F18" s="7">
         <v>100</v>
@@ -1121,7 +1134,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1129,13 +1142,14 @@
         <v>89.6</v>
       </c>
       <c r="C19" s="6">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D19" s="6">
         <v>3.1</v>
       </c>
       <c r="E19" s="7">
-        <f>D19*1000</f>
+        <f t="shared" si="0"/>
+        <v>3100</v>
       </c>
       <c r="F19" s="7">
         <v>100</v>
@@ -1147,7 +1161,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1161,7 +1175,8 @@
         <v>2.9</v>
       </c>
       <c r="E20" s="7">
-        <f>D20*1000</f>
+        <f t="shared" si="0"/>
+        <v>2900</v>
       </c>
       <c r="F20" s="7">
         <v>50</v>
@@ -1173,7 +1188,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1202,8 @@
         <v>2.6</v>
       </c>
       <c r="E21" s="7">
-        <f>D21*1000</f>
+        <f t="shared" si="0"/>
+        <v>2600</v>
       </c>
       <c r="F21" s="7">
         <v>50</v>
@@ -1199,7 +1215,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1213,7 +1229,8 @@
         <v>2.8</v>
       </c>
       <c r="E22" s="7">
-        <f>D22*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F22" s="7">
         <v>45</v>
@@ -1225,7 +1242,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1239,7 +1256,8 @@
         <v>2.8</v>
       </c>
       <c r="E23" s="7">
-        <f>D23*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F23" s="7">
         <v>30</v>
@@ -1251,7 +1269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1265,7 +1283,8 @@
         <v>2.4</v>
       </c>
       <c r="E24" s="7">
-        <f>D24*1000</f>
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
       <c r="F24" s="7">
         <v>50</v>
@@ -1277,7 +1296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1285,13 +1304,14 @@
         <v>20.8</v>
       </c>
       <c r="C25" s="6">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D25" s="6">
         <v>2.1</v>
       </c>
       <c r="E25" s="7">
-        <f>D25*1000</f>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="F25" s="7">
         <v>20</v>
@@ -1303,7 +1323,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1317,7 +1337,8 @@
         <v>2.5</v>
       </c>
       <c r="E26" s="7">
-        <f>D26*1000</f>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="F26" s="7">
         <v>20</v>
@@ -1329,7 +1350,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1343,7 +1364,8 @@
         <v>2.4</v>
       </c>
       <c r="E27" s="7">
-        <f>D27*1000</f>
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
       <c r="F27" s="7">
         <v>65</v>
@@ -1355,7 +1377,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1366,10 +1388,11 @@
         <v>16.8</v>
       </c>
       <c r="D28" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E28" s="7">
-        <f>D28*1000</f>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="F28" s="7">
         <v>65</v>
@@ -1381,7 +1404,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1418,8 @@
         <v>2.5</v>
       </c>
       <c r="E29" s="7">
-        <f>D29*1000</f>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="F29" s="7">
         <v>65</v>
@@ -1407,7 +1431,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1421,7 +1445,8 @@
         <v>2.5</v>
       </c>
       <c r="E30" s="7">
-        <f>D30*1000</f>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="F30" s="7">
         <v>20</v>
@@ -1433,7 +1458,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1441,13 +1466,14 @@
         <v>20.6</v>
       </c>
       <c r="C31" s="6">
-        <v>78.6</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="D31" s="6">
         <v>2.8</v>
       </c>
       <c r="E31" s="7">
-        <f>D31*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F31" s="7">
         <v>20</v>
@@ -1459,7 +1485,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1473,7 +1499,8 @@
         <v>2</v>
       </c>
       <c r="E32" s="7">
-        <f>D32*1000</f>
+        <f t="shared" si="0"/>
+        <v>2000</v>
       </c>
       <c r="F32" s="7">
         <v>100</v>
@@ -1485,7 +1512,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1499,7 +1526,8 @@
         <v>2.1</v>
       </c>
       <c r="E33" s="7">
-        <f>D33*1000</f>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="F33" s="7">
         <v>300</v>
@@ -1511,7 +1539,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1525,7 +1553,8 @@
         <v>2.5</v>
       </c>
       <c r="E34" s="7">
-        <f>D34*1000</f>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="F34" s="7">
         <v>145</v>
@@ -1537,7 +1566,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1545,13 +1574,14 @@
         <v>89.9</v>
       </c>
       <c r="C35" s="6">
-        <v>34.3</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D35" s="6">
         <v>2.7</v>
       </c>
       <c r="E35" s="7">
-        <f>D35*1000</f>
+        <f t="shared" si="0"/>
+        <v>2700</v>
       </c>
       <c r="F35" s="7">
         <v>130</v>
@@ -1563,7 +1593,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1577,7 +1607,8 @@
         <v>2.8</v>
       </c>
       <c r="E36" s="7">
-        <f>D36*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F36" s="7">
         <v>61</v>
@@ -1589,7 +1620,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1603,7 +1634,8 @@
         <v>2.8</v>
       </c>
       <c r="E37" s="7">
-        <f>D37*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F37" s="7">
         <v>40</v>
@@ -1615,7 +1647,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1626,10 +1658,11 @@
         <v>17.8</v>
       </c>
       <c r="D38" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E38" s="7">
-        <f>D38*1000</f>
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="F38" s="7">
         <v>50</v>
@@ -1641,7 +1674,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1655,7 +1688,8 @@
         <v>2.1</v>
       </c>
       <c r="E39" s="7">
-        <f>D39*1000</f>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="F39" s="7">
         <v>55</v>
@@ -1667,7 +1701,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -1681,7 +1715,8 @@
         <v>2.7</v>
       </c>
       <c r="E40" s="7">
-        <f>D40*1000</f>
+        <f t="shared" si="0"/>
+        <v>2700</v>
       </c>
       <c r="F40" s="7">
         <v>120</v>
@@ -1705,24 +1740,20 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView zoomScale="65" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:K40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>57</v>
       </c>
@@ -1757,7 +1788,7 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1771,10 +1802,11 @@
         <v>44.1</v>
       </c>
       <c r="E2" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F2" s="7">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F40" si="0">E2*1000</f>
+        <v>2300</v>
       </c>
       <c r="G2" s="7">
         <v>5</v>
@@ -1792,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1806,10 +1838,11 @@
         <v>59.5</v>
       </c>
       <c r="E3" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F3" s="7">
-        <f>E3*1000</f>
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="G3" s="7">
         <v>5</v>
@@ -1827,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1841,10 +1874,11 @@
         <v>51.4</v>
       </c>
       <c r="E4" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F4" s="7">
-        <f>E4*1000</f>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="G4" s="7">
         <v>5</v>
@@ -1862,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1873,13 +1907,14 @@
         <v>23</v>
       </c>
       <c r="D5" s="6">
-        <v>35.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="E5" s="6">
         <v>2.1</v>
       </c>
       <c r="F5" s="7">
-        <f>E5*1000</f>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G5" s="7">
         <v>5</v>
@@ -1897,7 +1932,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1905,16 +1940,17 @@
         <v>29.6</v>
       </c>
       <c r="C6" s="6">
-        <v>9.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D6" s="6">
         <v>58.5</v>
       </c>
       <c r="E6" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F6" s="7">
-        <f>E6*1000</f>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="G6" s="7">
         <v>10</v>
@@ -1932,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1946,10 +1982,11 @@
         <v>51.1</v>
       </c>
       <c r="E7" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F7" s="7">
-        <f>E7*1000</f>
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="G7" s="7">
         <v>5</v>
@@ -1967,7 +2004,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1978,13 +2015,14 @@
         <v>6.4</v>
       </c>
       <c r="D8" s="6">
-        <v>67.1</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="E8" s="6">
         <v>1.7</v>
       </c>
       <c r="F8" s="7">
-        <f>E8*1000</f>
+        <f t="shared" si="0"/>
+        <v>1700</v>
       </c>
       <c r="G8" s="7">
         <v>3</v>
@@ -2002,12 +2040,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C9" s="6">
         <v>11.6</v>
@@ -2016,10 +2054,11 @@
         <v>62.5</v>
       </c>
       <c r="E9" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F9" s="7">
-        <f>E9*1000</f>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="G9" s="7">
         <v>5</v>
@@ -2037,7 +2076,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2054,7 +2093,8 @@
         <v>1.5</v>
       </c>
       <c r="F10" s="7">
-        <f>E10*1000</f>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="G10" s="7">
         <v>17</v>
@@ -2072,7 +2112,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2089,7 +2129,8 @@
         <v>1.7</v>
       </c>
       <c r="F11" s="7">
-        <f>E11*1000</f>
+        <f t="shared" si="0"/>
+        <v>1700</v>
       </c>
       <c r="G11" s="7">
         <v>8</v>
@@ -2107,7 +2148,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2124,7 +2165,8 @@
         <v>1.5</v>
       </c>
       <c r="F12" s="7">
-        <f>E12*1000</f>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="G12" s="7">
         <v>5</v>
@@ -2142,7 +2184,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2159,7 +2201,8 @@
         <v>1.5</v>
       </c>
       <c r="F13" s="7">
-        <f>E13*1000</f>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="G13" s="7">
         <v>5</v>
@@ -2177,7 +2220,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2194,7 +2237,8 @@
         <v>1.8</v>
       </c>
       <c r="F14" s="7">
-        <f>E14*1000</f>
+        <f t="shared" si="0"/>
+        <v>1800</v>
       </c>
       <c r="G14" s="7">
         <v>5</v>
@@ -2212,7 +2256,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2223,13 +2267,14 @@
         <v>3.7</v>
       </c>
       <c r="D15" s="6">
-        <v>80.1</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="E15" s="6">
         <v>1.9</v>
       </c>
       <c r="F15" s="7">
-        <f>E15*1000</f>
+        <f t="shared" si="0"/>
+        <v>1900</v>
       </c>
       <c r="G15" s="7">
         <v>5</v>
@@ -2247,7 +2292,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2264,7 +2309,8 @@
         <v>1.5</v>
       </c>
       <c r="F16" s="7">
-        <f>E16*1000</f>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="G16" s="7">
         <v>15</v>
@@ -2282,7 +2328,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2299,7 +2345,8 @@
         <v>3.2</v>
       </c>
       <c r="F17" s="7">
-        <f>E17*1000</f>
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="G17" s="7">
         <v>75</v>
@@ -2317,7 +2364,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2328,13 +2375,14 @@
         <v>14.4</v>
       </c>
       <c r="D18" s="6">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="E18" s="6">
         <v>3.2</v>
       </c>
       <c r="F18" s="7">
-        <f>E18*1000</f>
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="G18" s="7">
         <v>100</v>
@@ -2352,7 +2400,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2360,7 +2408,7 @@
         <v>89.6</v>
       </c>
       <c r="C19" s="6">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D19" s="6">
         <v>11.2</v>
@@ -2369,7 +2417,8 @@
         <v>3.1</v>
       </c>
       <c r="F19" s="7">
-        <f>E19*1000</f>
+        <f t="shared" si="0"/>
+        <v>3100</v>
       </c>
       <c r="G19" s="7">
         <v>100</v>
@@ -2387,7 +2436,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2404,7 +2453,8 @@
         <v>2.9</v>
       </c>
       <c r="F20" s="7">
-        <f>E20*1000</f>
+        <f t="shared" si="0"/>
+        <v>2900</v>
       </c>
       <c r="G20" s="7">
         <v>50</v>
@@ -2422,7 +2472,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2439,7 +2489,8 @@
         <v>2.6</v>
       </c>
       <c r="F21" s="7">
-        <f>E21*1000</f>
+        <f t="shared" si="0"/>
+        <v>2600</v>
       </c>
       <c r="G21" s="7">
         <v>50</v>
@@ -2457,7 +2508,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2468,13 +2519,14 @@
         <v>15.9</v>
       </c>
       <c r="D22" s="6">
-        <v>39.8</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="E22" s="6">
         <v>2.8</v>
       </c>
       <c r="F22" s="7">
-        <f>E22*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G22" s="7">
         <v>45</v>
@@ -2492,7 +2544,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2509,7 +2561,8 @@
         <v>2.8</v>
       </c>
       <c r="F23" s="7">
-        <f>E23*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G23" s="7">
         <v>30</v>
@@ -2527,7 +2580,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2538,13 +2591,14 @@
         <v>10.7</v>
       </c>
       <c r="D24" s="6">
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="E24" s="6">
         <v>2.4</v>
       </c>
       <c r="F24" s="7">
-        <f>E24*1000</f>
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
       <c r="G24" s="7">
         <v>50</v>
@@ -2562,7 +2616,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2570,7 +2624,7 @@
         <v>20.8</v>
       </c>
       <c r="C25" s="6">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D25" s="6">
         <v>53.5</v>
@@ -2579,7 +2633,8 @@
         <v>2.1</v>
       </c>
       <c r="F25" s="7">
-        <f>E25*1000</f>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G25" s="7">
         <v>20</v>
@@ -2597,7 +2652,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2614,7 +2669,8 @@
         <v>2.5</v>
       </c>
       <c r="F26" s="7">
-        <f>E26*1000</f>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="G26" s="7">
         <v>20</v>
@@ -2632,7 +2688,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2649,7 +2705,8 @@
         <v>2.4</v>
       </c>
       <c r="F27" s="7">
-        <f>E27*1000</f>
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
       <c r="G27" s="7">
         <v>65</v>
@@ -2667,7 +2724,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -2681,10 +2738,11 @@
         <v>31.6</v>
       </c>
       <c r="E28" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F28" s="7">
-        <f>E28*1000</f>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="G28" s="7">
         <v>65</v>
@@ -2702,7 +2760,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -2719,7 +2777,8 @@
         <v>2.5</v>
       </c>
       <c r="F29" s="7">
-        <f>E29*1000</f>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="G29" s="7">
         <v>65</v>
@@ -2737,7 +2796,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -2754,7 +2813,8 @@
         <v>2.5</v>
       </c>
       <c r="F30" s="7">
-        <f>E30*1000</f>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="G30" s="7">
         <v>20</v>
@@ -2772,7 +2832,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2780,7 +2840,7 @@
         <v>20.6</v>
       </c>
       <c r="C31" s="6">
-        <v>78.6</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="D31" s="6">
         <v>13.3</v>
@@ -2789,7 +2849,8 @@
         <v>2.8</v>
       </c>
       <c r="F31" s="7">
-        <f>E31*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G31" s="7">
         <v>20</v>
@@ -2807,7 +2868,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -2824,7 +2885,8 @@
         <v>2</v>
       </c>
       <c r="F32" s="7">
-        <f>E32*1000</f>
+        <f t="shared" si="0"/>
+        <v>2000</v>
       </c>
       <c r="G32" s="7">
         <v>100</v>
@@ -2842,7 +2904,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -2853,13 +2915,14 @@
         <v>48</v>
       </c>
       <c r="D33" s="6">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="E33" s="6">
         <v>2.1</v>
       </c>
       <c r="F33" s="7">
-        <f>E33*1000</f>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G33" s="7">
         <v>300</v>
@@ -2877,7 +2940,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2894,7 +2957,8 @@
         <v>2.5</v>
       </c>
       <c r="F34" s="7">
-        <f>E34*1000</f>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="G34" s="7">
         <v>145</v>
@@ -2912,7 +2976,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
@@ -2920,16 +2984,17 @@
         <v>89.9</v>
       </c>
       <c r="C35" s="6">
-        <v>34.3</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D35" s="6">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="E35" s="6">
         <v>2.7</v>
       </c>
       <c r="F35" s="7">
-        <f>E35*1000</f>
+        <f t="shared" si="0"/>
+        <v>2700</v>
       </c>
       <c r="G35" s="7">
         <v>130</v>
@@ -2947,7 +3012,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2964,7 +3029,8 @@
         <v>2.8</v>
       </c>
       <c r="F36" s="7">
-        <f>E36*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G36" s="7">
         <v>61</v>
@@ -2982,7 +3048,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2999,7 +3065,8 @@
         <v>2.8</v>
       </c>
       <c r="F37" s="7">
-        <f>E37*1000</f>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G37" s="7">
         <v>40</v>
@@ -3017,7 +3084,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -3031,10 +3098,11 @@
         <v>57</v>
       </c>
       <c r="E38" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F38" s="7">
-        <f>E38*1000</f>
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="G38" s="7">
         <v>50</v>
@@ -3052,7 +3120,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -3069,7 +3137,8 @@
         <v>2.1</v>
       </c>
       <c r="F39" s="7">
-        <f>E39*1000</f>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G39" s="7">
         <v>55</v>
@@ -3087,7 +3156,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -3104,7 +3173,8 @@
         <v>2.7</v>
       </c>
       <c r="F40" s="7">
-        <f>E40*1000</f>
+        <f t="shared" si="0"/>
+        <v>2700</v>
       </c>
       <c r="G40" s="7">
         <v>120</v>
@@ -3129,27 +3199,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>57</v>
       </c>
@@ -3178,8 +3240,8 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6">
@@ -3192,10 +3254,11 @@
         <v>44.1</v>
       </c>
       <c r="E2" s="6">
-        <v>2.3</v>
-      </c>
-      <c r="F2" s="7">
-        <f>E2*1000</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F2" s="17">
+        <f t="shared" ref="F2:F40" si="0">E2*1000</f>
+        <v>2300</v>
       </c>
       <c r="G2" s="7">
         <v>5</v>
@@ -3204,11 +3267,11 @@
         <v>0.1</v>
       </c>
       <c r="I2" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6">
@@ -3221,10 +3284,11 @@
         <v>59.5</v>
       </c>
       <c r="E3" s="6">
-        <v>2.2</v>
-      </c>
-      <c r="F3" s="7">
-        <f>E3*1000</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="G3" s="7">
         <v>5</v>
@@ -3233,11 +3297,11 @@
         <v>0.1</v>
       </c>
       <c r="I3" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6">
@@ -3250,10 +3314,11 @@
         <v>51.4</v>
       </c>
       <c r="E4" s="6">
-        <v>2.3</v>
-      </c>
-      <c r="F4" s="7">
-        <f>E4*1000</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F4" s="17">
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="G4" s="7">
         <v>5</v>
@@ -3262,11 +3327,11 @@
         <v>0.1</v>
       </c>
       <c r="I4" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6">
@@ -3276,13 +3341,14 @@
         <v>23</v>
       </c>
       <c r="D5" s="6">
-        <v>35.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="E5" s="6">
         <v>2.1</v>
       </c>
-      <c r="F5" s="7">
-        <f>E5*1000</f>
+      <c r="F5" s="17">
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G5" s="7">
         <v>5</v>
@@ -3291,27 +3357,28 @@
         <v>0.1</v>
       </c>
       <c r="I5" s="6">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6">
         <v>29.6</v>
       </c>
       <c r="C6" s="6">
-        <v>9.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D6" s="6">
         <v>58.5</v>
       </c>
       <c r="E6" s="6">
-        <v>2.3</v>
-      </c>
-      <c r="F6" s="7">
-        <f>E6*1000</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F6" s="17">
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="G6" s="7">
         <v>10</v>
@@ -3320,11 +3387,11 @@
         <v>0.1</v>
       </c>
       <c r="I6" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6">
@@ -3337,10 +3404,11 @@
         <v>51.1</v>
       </c>
       <c r="E7" s="6">
-        <v>2.2</v>
-      </c>
-      <c r="F7" s="7">
-        <f>E7*1000</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F7" s="17">
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="G7" s="7">
         <v>5</v>
@@ -3349,11 +3417,11 @@
         <v>0.1</v>
       </c>
       <c r="I7" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="6">
@@ -3363,13 +3431,14 @@
         <v>6.4</v>
       </c>
       <c r="D8" s="6">
-        <v>67.1</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="E8" s="6">
         <v>1.7</v>
       </c>
-      <c r="F8" s="7">
-        <f>E8*1000</f>
+      <c r="F8" s="17">
+        <f t="shared" si="0"/>
+        <v>1700</v>
       </c>
       <c r="G8" s="7">
         <v>3</v>
@@ -3381,12 +3450,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C9" s="6">
         <v>11.6</v>
@@ -3395,10 +3464,11 @@
         <v>62.5</v>
       </c>
       <c r="E9" s="6">
-        <v>2.3</v>
-      </c>
-      <c r="F9" s="7">
-        <f>E9*1000</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F9" s="17">
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="G9" s="7">
         <v>5</v>
@@ -3407,11 +3477,11 @@
         <v>0.1</v>
       </c>
       <c r="I9" s="6">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="7">
@@ -3426,8 +3496,9 @@
       <c r="E10" s="6">
         <v>1.5</v>
       </c>
-      <c r="F10" s="7">
-        <f>E10*1000</f>
+      <c r="F10" s="17">
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="G10" s="7">
         <v>17</v>
@@ -3439,8 +3510,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6">
@@ -3455,8 +3526,9 @@
       <c r="E11" s="6">
         <v>1.7</v>
       </c>
-      <c r="F11" s="7">
-        <f>E11*1000</f>
+      <c r="F11" s="17">
+        <f t="shared" si="0"/>
+        <v>1700</v>
       </c>
       <c r="G11" s="7">
         <v>8</v>
@@ -3468,8 +3540,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="6">
@@ -3484,8 +3556,9 @@
       <c r="E12" s="6">
         <v>1.5</v>
       </c>
-      <c r="F12" s="7">
-        <f>E12*1000</f>
+      <c r="F12" s="17">
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="G12" s="7">
         <v>5</v>
@@ -3497,8 +3570,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="6">
@@ -3513,8 +3586,9 @@
       <c r="E13" s="6">
         <v>1.5</v>
       </c>
-      <c r="F13" s="7">
-        <f>E13*1000</f>
+      <c r="F13" s="17">
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="G13" s="7">
         <v>5</v>
@@ -3526,8 +3600,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="6">
@@ -3542,8 +3616,9 @@
       <c r="E14" s="6">
         <v>1.8</v>
       </c>
-      <c r="F14" s="7">
-        <f>E14*1000</f>
+      <c r="F14" s="17">
+        <f t="shared" si="0"/>
+        <v>1800</v>
       </c>
       <c r="G14" s="7">
         <v>5</v>
@@ -3555,8 +3630,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="6">
@@ -3566,13 +3641,14 @@
         <v>3.7</v>
       </c>
       <c r="D15" s="6">
-        <v>80.1</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="E15" s="6">
         <v>1.9</v>
       </c>
-      <c r="F15" s="7">
-        <f>E15*1000</f>
+      <c r="F15" s="17">
+        <f t="shared" si="0"/>
+        <v>1900</v>
       </c>
       <c r="G15" s="7">
         <v>5</v>
@@ -3584,8 +3660,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="6">
@@ -3600,8 +3676,9 @@
       <c r="E16" s="6">
         <v>1.5</v>
       </c>
-      <c r="F16" s="7">
-        <f>E16*1000</f>
+      <c r="F16" s="17">
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="G16" s="7">
         <v>15</v>
@@ -3613,8 +3690,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="6">
@@ -3629,8 +3706,9 @@
       <c r="E17" s="6">
         <v>3.2</v>
       </c>
-      <c r="F17" s="7">
-        <f>E17*1000</f>
+      <c r="F17" s="17">
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="G17" s="7">
         <v>75</v>
@@ -3642,8 +3720,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="7">
@@ -3653,13 +3731,14 @@
         <v>14.4</v>
       </c>
       <c r="D18" s="6">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="E18" s="6">
         <v>3.2</v>
       </c>
-      <c r="F18" s="7">
-        <f>E18*1000</f>
+      <c r="F18" s="17">
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="G18" s="7">
         <v>100</v>
@@ -3671,15 +3750,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="6">
         <v>89.6</v>
       </c>
       <c r="C19" s="6">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D19" s="6">
         <v>11.2</v>
@@ -3687,8 +3766,9 @@
       <c r="E19" s="6">
         <v>3.1</v>
       </c>
-      <c r="F19" s="7">
-        <f>E19*1000</f>
+      <c r="F19" s="17">
+        <f t="shared" si="0"/>
+        <v>3100</v>
       </c>
       <c r="G19" s="7">
         <v>100</v>
@@ -3700,8 +3780,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="6">
@@ -3716,8 +3796,9 @@
       <c r="E20" s="6">
         <v>2.9</v>
       </c>
-      <c r="F20" s="7">
-        <f>E20*1000</f>
+      <c r="F20" s="17">
+        <f t="shared" si="0"/>
+        <v>2900</v>
       </c>
       <c r="G20" s="7">
         <v>50</v>
@@ -3729,8 +3810,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="7">
@@ -3745,8 +3826,9 @@
       <c r="E21" s="6">
         <v>2.6</v>
       </c>
-      <c r="F21" s="7">
-        <f>E21*1000</f>
+      <c r="F21" s="17">
+        <f t="shared" si="0"/>
+        <v>2600</v>
       </c>
       <c r="G21" s="7">
         <v>50</v>
@@ -3758,8 +3840,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="7">
@@ -3769,13 +3851,14 @@
         <v>15.9</v>
       </c>
       <c r="D22" s="6">
-        <v>39.8</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="E22" s="6">
         <v>2.8</v>
       </c>
-      <c r="F22" s="7">
-        <f>E22*1000</f>
+      <c r="F22" s="17">
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G22" s="7">
         <v>45</v>
@@ -3787,8 +3870,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="6">
@@ -3803,8 +3886,9 @@
       <c r="E23" s="6">
         <v>2.8</v>
       </c>
-      <c r="F23" s="7">
-        <f>E23*1000</f>
+      <c r="F23" s="17">
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G23" s="7">
         <v>30</v>
@@ -3816,8 +3900,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="7">
@@ -3827,13 +3911,14 @@
         <v>10.7</v>
       </c>
       <c r="D24" s="6">
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="E24" s="6">
         <v>2.4</v>
       </c>
-      <c r="F24" s="7">
-        <f>E24*1000</f>
+      <c r="F24" s="17">
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
       <c r="G24" s="7">
         <v>50</v>
@@ -3845,15 +3930,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="6">
         <v>20.8</v>
       </c>
       <c r="C25" s="6">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D25" s="6">
         <v>53.5</v>
@@ -3861,8 +3946,9 @@
       <c r="E25" s="6">
         <v>2.1</v>
       </c>
-      <c r="F25" s="7">
-        <f>E25*1000</f>
+      <c r="F25" s="17">
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G25" s="7">
         <v>20</v>
@@ -3874,8 +3960,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="7">
@@ -3890,8 +3976,9 @@
       <c r="E26" s="6">
         <v>2.5</v>
       </c>
-      <c r="F26" s="7">
-        <f>E26*1000</f>
+      <c r="F26" s="17">
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="G26" s="7">
         <v>20</v>
@@ -3903,8 +3990,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="7">
@@ -3919,8 +4006,9 @@
       <c r="E27" s="6">
         <v>2.4</v>
       </c>
-      <c r="F27" s="7">
-        <f>E27*1000</f>
+      <c r="F27" s="17">
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
       <c r="G27" s="7">
         <v>65</v>
@@ -3932,8 +4020,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="6">
@@ -3946,10 +4034,11 @@
         <v>31.6</v>
       </c>
       <c r="E28" s="6">
-        <v>2.3</v>
-      </c>
-      <c r="F28" s="7">
-        <f>E28*1000</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F28" s="17">
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="G28" s="7">
         <v>65</v>
@@ -3961,8 +4050,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="6">
@@ -3977,8 +4066,9 @@
       <c r="E29" s="6">
         <v>2.5</v>
       </c>
-      <c r="F29" s="7">
-        <f>E29*1000</f>
+      <c r="F29" s="17">
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="G29" s="7">
         <v>65</v>
@@ -3990,8 +4080,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="7">
@@ -4006,8 +4096,9 @@
       <c r="E30" s="6">
         <v>2.5</v>
       </c>
-      <c r="F30" s="7">
-        <f>E30*1000</f>
+      <c r="F30" s="17">
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="G30" s="7">
         <v>20</v>
@@ -4019,15 +4110,15 @@
         <v>0.09</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="6">
         <v>20.6</v>
       </c>
       <c r="C31" s="6">
-        <v>78.6</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="D31" s="6">
         <v>13.3</v>
@@ -4035,8 +4126,9 @@
       <c r="E31" s="6">
         <v>2.8</v>
       </c>
-      <c r="F31" s="7">
-        <f>E31*1000</f>
+      <c r="F31" s="17">
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G31" s="7">
         <v>20</v>
@@ -4048,8 +4140,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="6">
@@ -4064,8 +4156,9 @@
       <c r="E32" s="7">
         <v>2</v>
       </c>
-      <c r="F32" s="7">
-        <f>E32*1000</f>
+      <c r="F32" s="17">
+        <f t="shared" si="0"/>
+        <v>2000</v>
       </c>
       <c r="G32" s="7">
         <v>100</v>
@@ -4077,8 +4170,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="6">
@@ -4088,13 +4181,14 @@
         <v>48</v>
       </c>
       <c r="D33" s="6">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="E33" s="6">
         <v>2.1</v>
       </c>
-      <c r="F33" s="7">
-        <f>E33*1000</f>
+      <c r="F33" s="17">
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G33" s="7">
         <v>300</v>
@@ -4106,8 +4200,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="6">
@@ -4122,8 +4216,9 @@
       <c r="E34" s="6">
         <v>2.5</v>
       </c>
-      <c r="F34" s="7">
-        <f>E34*1000</f>
+      <c r="F34" s="17">
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="G34" s="7">
         <v>145</v>
@@ -4135,24 +4230,25 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B35" s="6">
         <v>89.9</v>
       </c>
       <c r="C35" s="6">
-        <v>34.3</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D35" s="6">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="E35" s="6">
         <v>2.7</v>
       </c>
-      <c r="F35" s="7">
-        <f>E35*1000</f>
+      <c r="F35" s="17">
+        <f t="shared" si="0"/>
+        <v>2700</v>
       </c>
       <c r="G35" s="7">
         <v>130</v>
@@ -4164,8 +4260,8 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="6">
@@ -4180,8 +4276,9 @@
       <c r="E36" s="6">
         <v>2.8</v>
       </c>
-      <c r="F36" s="7">
-        <f>E36*1000</f>
+      <c r="F36" s="17">
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G36" s="7">
         <v>61</v>
@@ -4193,8 +4290,8 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="7">
@@ -4209,8 +4306,9 @@
       <c r="E37" s="6">
         <v>2.8</v>
       </c>
-      <c r="F37" s="7">
-        <f>E37*1000</f>
+      <c r="F37" s="17">
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G37" s="7">
         <v>40</v>
@@ -4222,8 +4320,8 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="6">
@@ -4236,10 +4334,11 @@
         <v>57</v>
       </c>
       <c r="E38" s="6">
-        <v>2.2</v>
-      </c>
-      <c r="F38" s="7">
-        <f>E38*1000</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F38" s="17">
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="G38" s="7">
         <v>50</v>
@@ -4251,8 +4350,8 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="7">
@@ -4267,8 +4366,9 @@
       <c r="E39" s="6">
         <v>2.1</v>
       </c>
-      <c r="F39" s="7">
-        <f>E39*1000</f>
+      <c r="F39" s="17">
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G39" s="7">
         <v>55</v>
@@ -4280,8 +4380,8 @@
         <v>0.25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="7">
@@ -4296,8 +4396,9 @@
       <c r="E40" s="6">
         <v>2.7</v>
       </c>
-      <c r="F40" s="7">
-        <f>E40*1000</f>
+      <c r="F40" s="17">
+        <f t="shared" si="0"/>
+        <v>2700</v>
       </c>
       <c r="G40" s="7">
         <v>120</v>
@@ -4321,20 +4422,20 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -4357,7 +4458,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -4372,13 +4473,13 @@
         <v>23.5</v>
       </c>
       <c r="F2" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G2" s="7">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -4393,13 +4494,13 @@
         <v>8.9</v>
       </c>
       <c r="F3" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G3" s="7">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -4414,13 +4515,13 @@
         <v>14.2</v>
       </c>
       <c r="F4" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G4" s="7">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -4441,7 +4542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -4453,16 +4554,16 @@
         <v>62.6</v>
       </c>
       <c r="E6" s="6">
-        <v>9.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="F6" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G6" s="7">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -4477,13 +4578,13 @@
         <v>4</v>
       </c>
       <c r="F7" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G7" s="7">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -4504,13 +4605,13 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="6">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="D9" s="6">
         <v>62.3</v>
@@ -4519,13 +4620,13 @@
         <v>11.6</v>
       </c>
       <c r="F9" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G9" s="7">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>46</v>
@@ -4538,7 +4639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
@@ -4551,7 +4652,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -4572,7 +4673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -4593,7 +4694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -4614,7 +4715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -4635,7 +4736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -4656,7 +4757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -4677,7 +4778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
@@ -4698,7 +4799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
@@ -4711,7 +4812,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>15</v>
@@ -4732,7 +4833,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>16</v>
@@ -4753,7 +4854,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>17</v>
@@ -4765,7 +4866,7 @@
         <v>86.7</v>
       </c>
       <c r="E22" s="6">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="F22" s="6">
         <v>3.1</v>
@@ -4774,7 +4875,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>18</v>
@@ -4795,7 +4896,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>19</v>
@@ -4804,7 +4905,7 @@
         <v>89</v>
       </c>
       <c r="D24" s="6">
-        <v>73.1</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="E24" s="7">
         <v>10</v>
@@ -4816,7 +4917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>20</v>
@@ -4825,7 +4926,7 @@
         <v>87</v>
       </c>
       <c r="D25" s="6">
-        <v>78.1</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E25" s="6">
         <v>15.9</v>
@@ -4837,7 +4938,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>21</v>
@@ -4846,7 +4947,7 @@
         <v>90.2</v>
       </c>
       <c r="D26" s="6">
-        <v>76.4</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="E26" s="6">
         <v>15.9</v>
@@ -4858,7 +4959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>22</v>
@@ -4867,7 +4968,7 @@
         <v>21</v>
       </c>
       <c r="D27" s="6">
-        <v>66.1</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="E27" s="6">
         <v>10.7</v>
@@ -4879,7 +4980,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>23</v>
@@ -4891,7 +4992,7 @@
         <v>57.4</v>
       </c>
       <c r="E28" s="6">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="F28" s="6">
         <v>2.1</v>
@@ -4900,7 +5001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>24</v>
@@ -4921,7 +5022,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>25</v>
@@ -4930,7 +5031,7 @@
         <v>89</v>
       </c>
       <c r="D30" s="6">
-        <v>65.1</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="E30" s="6">
         <v>15.3</v>
@@ -4942,7 +5043,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>26</v>
@@ -4957,13 +5058,13 @@
         <v>16.8</v>
       </c>
       <c r="F31" s="6">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G31" s="7">
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>27</v>
@@ -4984,7 +5085,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>28</v>
@@ -5005,7 +5106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>29</v>
@@ -5017,7 +5118,7 @@
         <v>12.3</v>
       </c>
       <c r="E34" s="6">
-        <v>78.6</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="F34" s="6">
         <v>2.8</v>
@@ -5026,7 +5127,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>51</v>
       </c>
@@ -5039,7 +5140,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
         <v>30</v>
@@ -5060,7 +5161,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>31</v>
@@ -5081,7 +5182,7 @@
         <v>300</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>32</v>
@@ -5090,7 +5191,7 @@
         <v>88.8</v>
       </c>
       <c r="D38" s="6">
-        <v>70.1</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="E38" s="6">
         <v>39.6</v>
@@ -5102,7 +5203,7 @@
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>33</v>
@@ -5114,7 +5215,7 @@
         <v>73.5</v>
       </c>
       <c r="E39" s="6">
-        <v>34.3</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="F39" s="6">
         <v>2.7</v>
@@ -5123,7 +5224,7 @@
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>34</v>
@@ -5144,7 +5245,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>35</v>
@@ -5153,7 +5254,7 @@
         <v>90</v>
       </c>
       <c r="D41" s="6">
-        <v>78.1</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E41" s="6">
         <v>59.7</v>
@@ -5165,7 +5266,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>36</v>
@@ -5180,13 +5281,13 @@
         <v>17.8</v>
       </c>
       <c r="F42" s="6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G42" s="7">
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>37</v>
@@ -5207,7 +5308,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>38</v>
@@ -5228,7 +5329,7 @@
         <v>120</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
@@ -5241,7 +5342,7 @@
       <c r="F45" s="9"/>
       <c r="G45" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
         <v>55</v>
@@ -5254,7 +5355,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
         <v>56</v>
@@ -5270,336 +5371,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>